<commit_message>
continued working on PJ4
</commit_message>
<xml_diff>
--- a/Copy of earnings_Alnylam.xlsx
+++ b/Copy of earnings_Alnylam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianweissmeier/Documents/Wu_Wien/Q3/Corporate Finance/Team_Project/r-code/Corporate Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54495DDA-CC85-994F-990A-610334B3BD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDADBFF5-CC7B-C345-A62E-E6CAF93F7A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Per</t>
   </si>
@@ -46,15 +46,6 @@
   </si>
   <si>
     <t>Estimate</t>
-  </si>
-  <si>
-    <t>02/13/2025</t>
-  </si>
-  <si>
-    <t>Q4 24</t>
-  </si>
-  <si>
-    <t>12/24</t>
   </si>
   <si>
     <t>10/31/2024</t>
@@ -849,13 +840,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>198967</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1228,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1257,10 +1248,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,18 +1265,18 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>-0.65</v>
+        <v>-0.87</v>
       </c>
       <c r="E2">
-        <v>-0.64200000000000002</v>
+        <v>-0.94399999999999995</v>
       </c>
       <c r="F2" s="2">
-        <f>+(D2-E2)/ABS(D2)</f>
-        <v>-1.2307692307692318E-2</v>
+        <f t="shared" ref="F2:F24" si="0">+(D2-E2)/ABS(D2)</f>
+        <v>8.5057471264367759E-2</v>
       </c>
       <c r="G2" t="str">
-        <f>+IF(F2&gt;=0.025,"Good",IF(F2&lt;=-0.025,"Bad","Neutral"))</f>
-        <v>Neutral</v>
+        <f t="shared" ref="G2:G24" si="1">+IF(F2&gt;=0.025,"Good",IF(F2&lt;=-0.025,"Bad","Neutral"))</f>
+        <v>Good</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1299,17 +1290,17 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>-0.87</v>
+        <v>-0.13</v>
       </c>
       <c r="E3">
-        <v>-0.94399999999999995</v>
+        <v>-1.0649999999999999</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F25" si="0">+(D3-E3)/ABS(D3)</f>
-        <v>8.5057471264367759E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1923076923076916</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G2:G25" si="1">+IF(F3&gt;=0.025,"Good",IF(F3&lt;=-0.025,"Bad","Neutral"))</f>
+        <f t="shared" si="1"/>
         <v>Good</v>
       </c>
     </row>
@@ -1324,14 +1315,14 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>-0.13</v>
+        <v>-0.52</v>
       </c>
       <c r="E4">
-        <v>-1.0649999999999999</v>
+        <v>-1.196</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>7.1923076923076916</v>
+        <v>1.2999999999999998</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -1349,14 +1340,14 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>-0.52</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E5">
-        <v>-1.196</v>
+        <v>-1.256</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>1.2999999999999998</v>
+        <v>0.14181818181818173</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -1374,14 +1365,14 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>-1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E6">
-        <v>-1.256</v>
+        <v>-1.538</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>0.14181818181818173</v>
+        <v>2.3373913043478258</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -1399,18 +1390,18 @@
         <v>21</v>
       </c>
       <c r="D7">
-        <v>1.1499999999999999</v>
+        <v>-2.21</v>
       </c>
       <c r="E7">
-        <v>-1.538</v>
+        <v>-1.516</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>2.3373913043478258</v>
+        <v>-0.31402714932126696</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1424,18 +1415,18 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>-2.21</v>
+        <v>-1.4</v>
       </c>
       <c r="E8">
-        <v>-1.516</v>
+        <v>-1.7709999999999999</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>-0.31402714932126696</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1449,14 +1440,14 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>-1.4</v>
+        <v>-1.68</v>
       </c>
       <c r="E9">
-        <v>-1.7709999999999999</v>
+        <v>-1.9119999999999999</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.26500000000000001</v>
+        <v>0.1380952380952381</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -1474,18 +1465,18 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>-1.68</v>
+        <v>-3.32</v>
       </c>
       <c r="E10">
-        <v>-1.9119999999999999</v>
+        <v>-1.79</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>0.1380952380952381</v>
+        <v>-0.46084337349397586</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1499,14 +1490,14 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>-3.32</v>
+        <v>-2.29</v>
       </c>
       <c r="E11">
-        <v>-1.79</v>
+        <v>-1.7130000000000001</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>-0.46084337349397586</v>
+        <v>-0.25196506550218339</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -1524,14 +1515,14 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>-2.29</v>
+        <v>-2</v>
       </c>
       <c r="E12">
-        <v>-1.7130000000000001</v>
+        <v>-1.9239999999999999</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>-0.25196506550218339</v>
+        <v>-3.8000000000000034E-2</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -1549,14 +1540,14 @@
         <v>39</v>
       </c>
       <c r="D13">
-        <v>-2</v>
+        <v>-2.16</v>
       </c>
       <c r="E13">
-        <v>-1.9239999999999999</v>
+        <v>-1.474</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>-3.8000000000000034E-2</v>
+        <v>-0.31759259259259265</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -1574,14 +1565,14 @@
         <v>42</v>
       </c>
       <c r="D14">
-        <v>-2.16</v>
+        <v>-1.72</v>
       </c>
       <c r="E14">
-        <v>-1.474</v>
+        <v>-1.5229999999999999</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>-0.31759259259259265</v>
+        <v>-0.11453488372093028</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -1599,18 +1590,18 @@
         <v>45</v>
       </c>
       <c r="D15">
-        <v>-1.72</v>
+        <v>-1.61</v>
       </c>
       <c r="E15">
-        <v>-1.5229999999999999</v>
+        <v>-1.625</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>-0.11453488372093028</v>
+        <v>9.3167701863353432E-3</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Neutral</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1624,18 +1615,18 @@
         <v>48</v>
       </c>
       <c r="D16">
-        <v>-1.61</v>
+        <v>-1.71</v>
       </c>
       <c r="E16">
-        <v>-1.625</v>
+        <v>-1.7629999999999999</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>9.3167701863353432E-3</v>
+        <v>3.0994152046783588E-2</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>Neutral</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1649,18 +1640,18 @@
         <v>51</v>
       </c>
       <c r="D17">
-        <v>-1.71</v>
+        <v>-2.09</v>
       </c>
       <c r="E17">
-        <v>-1.7629999999999999</v>
+        <v>-1.7410000000000001</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>3.0994152046783588E-2</v>
+        <v>-0.16698564593301424</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1674,14 +1665,14 @@
         <v>54</v>
       </c>
       <c r="D18">
-        <v>-2.09</v>
+        <v>-2.1800000000000002</v>
       </c>
       <c r="E18">
-        <v>-1.7410000000000001</v>
+        <v>-1.599</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.16698564593301424</v>
+        <v>-0.26651376146788996</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
@@ -1699,18 +1690,18 @@
         <v>57</v>
       </c>
       <c r="D19">
-        <v>-2.1800000000000002</v>
+        <v>-1.56</v>
       </c>
       <c r="E19">
-        <v>-1.599</v>
+        <v>-1.8069999999999999</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>-0.26651376146788996</v>
+        <v>0.15833333333333324</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1724,14 +1715,14 @@
         <v>60</v>
       </c>
       <c r="D20">
-        <v>-1.56</v>
+        <v>-1.62</v>
       </c>
       <c r="E20">
-        <v>-1.8069999999999999</v>
+        <v>-1.8520000000000001</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>0.15833333333333324</v>
+        <v>0.14320987654320985</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
@@ -1749,18 +1740,18 @@
         <v>63</v>
       </c>
       <c r="D21">
-        <v>-1.62</v>
+        <v>-2.4700000000000002</v>
       </c>
       <c r="E21">
-        <v>-1.8520000000000001</v>
+        <v>-2.2210000000000001</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>0.14320987654320985</v>
+        <v>-0.10080971659919032</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1774,18 +1765,18 @@
         <v>66</v>
       </c>
       <c r="D22">
-        <v>-2.4700000000000002</v>
+        <v>-1.92</v>
       </c>
       <c r="E22">
-        <v>-2.2210000000000001</v>
+        <v>-2.121</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
-        <v>-0.10080971659919032</v>
+        <v>0.10468750000000004</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,14 +1790,14 @@
         <v>69</v>
       </c>
       <c r="D23">
-        <v>-1.92</v>
+        <v>-2.02</v>
       </c>
       <c r="E23">
-        <v>-2.121</v>
+        <v>-2.12</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
-        <v>0.10468750000000004</v>
+        <v>4.9504950495049549E-2</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -1824,14 +1815,14 @@
         <v>72</v>
       </c>
       <c r="D24">
-        <v>-2.02</v>
+        <v>-1.73</v>
       </c>
       <c r="E24">
-        <v>-2.12</v>
+        <v>-2.0859999999999999</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
-        <v>4.9504950495049549E-2</v>
+        <v>0.20578034682080917</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -1839,29 +1830,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25">
-        <v>-1.73</v>
-      </c>
-      <c r="E25">
-        <v>-2.0859999999999999</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20578034682080917</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>Good</v>
-      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F26" s="2"/>
@@ -1919,9 +1888,6 @@
     </row>
     <row r="44" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,28 +1907,28 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B4)</f>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B4)</f>
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B5)</f>
-        <v>2</v>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B6)</f>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B6)</f>
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code and data
</commit_message>
<xml_diff>
--- a/Copy of earnings_Alnylam.xlsx
+++ b/Copy of earnings_Alnylam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianweissmeier/Documents/Wu_Wien/Q3/Corporate Finance/Team_Project/r-code/Corporate Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54495DDA-CC85-994F-990A-610334B3BD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDADBFF5-CC7B-C345-A62E-E6CAF93F7A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Per</t>
   </si>
@@ -46,15 +46,6 @@
   </si>
   <si>
     <t>Estimate</t>
-  </si>
-  <si>
-    <t>02/13/2025</t>
-  </si>
-  <si>
-    <t>Q4 24</t>
-  </si>
-  <si>
-    <t>12/24</t>
   </si>
   <si>
     <t>10/31/2024</t>
@@ -849,13 +840,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>198967</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1228,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1233,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1257,10 +1248,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1274,18 +1265,18 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>-0.65</v>
+        <v>-0.87</v>
       </c>
       <c r="E2">
-        <v>-0.64200000000000002</v>
+        <v>-0.94399999999999995</v>
       </c>
       <c r="F2" s="2">
-        <f>+(D2-E2)/ABS(D2)</f>
-        <v>-1.2307692307692318E-2</v>
+        <f t="shared" ref="F2:F24" si="0">+(D2-E2)/ABS(D2)</f>
+        <v>8.5057471264367759E-2</v>
       </c>
       <c r="G2" t="str">
-        <f>+IF(F2&gt;=0.025,"Good",IF(F2&lt;=-0.025,"Bad","Neutral"))</f>
-        <v>Neutral</v>
+        <f t="shared" ref="G2:G24" si="1">+IF(F2&gt;=0.025,"Good",IF(F2&lt;=-0.025,"Bad","Neutral"))</f>
+        <v>Good</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1299,17 +1290,17 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>-0.87</v>
+        <v>-0.13</v>
       </c>
       <c r="E3">
-        <v>-0.94399999999999995</v>
+        <v>-1.0649999999999999</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F25" si="0">+(D3-E3)/ABS(D3)</f>
-        <v>8.5057471264367759E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.1923076923076916</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G2:G25" si="1">+IF(F3&gt;=0.025,"Good",IF(F3&lt;=-0.025,"Bad","Neutral"))</f>
+        <f t="shared" si="1"/>
         <v>Good</v>
       </c>
     </row>
@@ -1324,14 +1315,14 @@
         <v>12</v>
       </c>
       <c r="D4">
-        <v>-0.13</v>
+        <v>-0.52</v>
       </c>
       <c r="E4">
-        <v>-1.0649999999999999</v>
+        <v>-1.196</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>7.1923076923076916</v>
+        <v>1.2999999999999998</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -1349,14 +1340,14 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>-0.52</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="E5">
-        <v>-1.196</v>
+        <v>-1.256</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>1.2999999999999998</v>
+        <v>0.14181818181818173</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -1374,14 +1365,14 @@
         <v>18</v>
       </c>
       <c r="D6">
-        <v>-1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="E6">
-        <v>-1.256</v>
+        <v>-1.538</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>0.14181818181818173</v>
+        <v>2.3373913043478258</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -1399,18 +1390,18 @@
         <v>21</v>
       </c>
       <c r="D7">
-        <v>1.1499999999999999</v>
+        <v>-2.21</v>
       </c>
       <c r="E7">
-        <v>-1.538</v>
+        <v>-1.516</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>2.3373913043478258</v>
+        <v>-0.31402714932126696</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1424,18 +1415,18 @@
         <v>24</v>
       </c>
       <c r="D8">
-        <v>-2.21</v>
+        <v>-1.4</v>
       </c>
       <c r="E8">
-        <v>-1.516</v>
+        <v>-1.7709999999999999</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>-0.31402714932126696</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1449,14 +1440,14 @@
         <v>27</v>
       </c>
       <c r="D9">
-        <v>-1.4</v>
+        <v>-1.68</v>
       </c>
       <c r="E9">
-        <v>-1.7709999999999999</v>
+        <v>-1.9119999999999999</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.26500000000000001</v>
+        <v>0.1380952380952381</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -1474,18 +1465,18 @@
         <v>30</v>
       </c>
       <c r="D10">
-        <v>-1.68</v>
+        <v>-3.32</v>
       </c>
       <c r="E10">
-        <v>-1.9119999999999999</v>
+        <v>-1.79</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>0.1380952380952381</v>
+        <v>-0.46084337349397586</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1499,14 +1490,14 @@
         <v>33</v>
       </c>
       <c r="D11">
-        <v>-3.32</v>
+        <v>-2.29</v>
       </c>
       <c r="E11">
-        <v>-1.79</v>
+        <v>-1.7130000000000001</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>-0.46084337349397586</v>
+        <v>-0.25196506550218339</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -1524,14 +1515,14 @@
         <v>36</v>
       </c>
       <c r="D12">
-        <v>-2.29</v>
+        <v>-2</v>
       </c>
       <c r="E12">
-        <v>-1.7130000000000001</v>
+        <v>-1.9239999999999999</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>-0.25196506550218339</v>
+        <v>-3.8000000000000034E-2</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -1549,14 +1540,14 @@
         <v>39</v>
       </c>
       <c r="D13">
-        <v>-2</v>
+        <v>-2.16</v>
       </c>
       <c r="E13">
-        <v>-1.9239999999999999</v>
+        <v>-1.474</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>-3.8000000000000034E-2</v>
+        <v>-0.31759259259259265</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -1574,14 +1565,14 @@
         <v>42</v>
       </c>
       <c r="D14">
-        <v>-2.16</v>
+        <v>-1.72</v>
       </c>
       <c r="E14">
-        <v>-1.474</v>
+        <v>-1.5229999999999999</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>-0.31759259259259265</v>
+        <v>-0.11453488372093028</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -1599,18 +1590,18 @@
         <v>45</v>
       </c>
       <c r="D15">
-        <v>-1.72</v>
+        <v>-1.61</v>
       </c>
       <c r="E15">
-        <v>-1.5229999999999999</v>
+        <v>-1.625</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>-0.11453488372093028</v>
+        <v>9.3167701863353432E-3</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Neutral</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1624,18 +1615,18 @@
         <v>48</v>
       </c>
       <c r="D16">
-        <v>-1.61</v>
+        <v>-1.71</v>
       </c>
       <c r="E16">
-        <v>-1.625</v>
+        <v>-1.7629999999999999</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>9.3167701863353432E-3</v>
+        <v>3.0994152046783588E-2</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>Neutral</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1649,18 +1640,18 @@
         <v>51</v>
       </c>
       <c r="D17">
-        <v>-1.71</v>
+        <v>-2.09</v>
       </c>
       <c r="E17">
-        <v>-1.7629999999999999</v>
+        <v>-1.7410000000000001</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>3.0994152046783588E-2</v>
+        <v>-0.16698564593301424</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1674,14 +1665,14 @@
         <v>54</v>
       </c>
       <c r="D18">
-        <v>-2.09</v>
+        <v>-2.1800000000000002</v>
       </c>
       <c r="E18">
-        <v>-1.7410000000000001</v>
+        <v>-1.599</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>-0.16698564593301424</v>
+        <v>-0.26651376146788996</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
@@ -1699,18 +1690,18 @@
         <v>57</v>
       </c>
       <c r="D19">
-        <v>-2.1800000000000002</v>
+        <v>-1.56</v>
       </c>
       <c r="E19">
-        <v>-1.599</v>
+        <v>-1.8069999999999999</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>-0.26651376146788996</v>
+        <v>0.15833333333333324</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1724,14 +1715,14 @@
         <v>60</v>
       </c>
       <c r="D20">
-        <v>-1.56</v>
+        <v>-1.62</v>
       </c>
       <c r="E20">
-        <v>-1.8069999999999999</v>
+        <v>-1.8520000000000001</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>0.15833333333333324</v>
+        <v>0.14320987654320985</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
@@ -1749,18 +1740,18 @@
         <v>63</v>
       </c>
       <c r="D21">
-        <v>-1.62</v>
+        <v>-2.4700000000000002</v>
       </c>
       <c r="E21">
-        <v>-1.8520000000000001</v>
+        <v>-2.2210000000000001</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>0.14320987654320985</v>
+        <v>-0.10080971659919032</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
+        <v>Bad</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1774,18 +1765,18 @@
         <v>66</v>
       </c>
       <c r="D22">
-        <v>-2.4700000000000002</v>
+        <v>-1.92</v>
       </c>
       <c r="E22">
-        <v>-2.2210000000000001</v>
+        <v>-2.121</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
-        <v>-0.10080971659919032</v>
+        <v>0.10468750000000004</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
+        <v>Good</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1799,14 +1790,14 @@
         <v>69</v>
       </c>
       <c r="D23">
-        <v>-1.92</v>
+        <v>-2.02</v>
       </c>
       <c r="E23">
-        <v>-2.121</v>
+        <v>-2.12</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="0"/>
-        <v>0.10468750000000004</v>
+        <v>4.9504950495049549E-2</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -1824,14 +1815,14 @@
         <v>72</v>
       </c>
       <c r="D24">
-        <v>-2.02</v>
+        <v>-1.73</v>
       </c>
       <c r="E24">
-        <v>-2.12</v>
+        <v>-2.0859999999999999</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="0"/>
-        <v>4.9504950495049549E-2</v>
+        <v>0.20578034682080917</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -1839,29 +1830,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25">
-        <v>-1.73</v>
-      </c>
-      <c r="E25">
-        <v>-2.0859999999999999</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.20578034682080917</v>
-      </c>
-      <c r="G25" t="str">
-        <f t="shared" si="1"/>
-        <v>Good</v>
-      </c>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="F26" s="2"/>
@@ -1919,9 +1888,6 @@
     </row>
     <row r="44" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1941,28 +1907,28 @@
   <sheetData>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B4)</f>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B4)</f>
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B5)</f>
-        <v>2</v>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C6">
-        <f>+COUNTIF(Worksheet!$G$2:$G$25,Formula!B6)</f>
+        <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B6)</f>
         <v>9</v>
       </c>
     </row>
@@ -1970,4 +1936,175 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006483248081D4D34083215F2A9507A283" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e618be4f2b80e79eaadc52ea446d95c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="85942912-2c17-4d13-bcab-472c0bf30a39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c80daec75caaa22acc5c26d2fb929cb0" ns2:_="">
+    <xsd:import namespace="85942912-2c17-4d13-bcab-472c0bf30a39"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="85942912-2c17-4d13-bcab-472c0bf30a39" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56694664-2CCF-469C-A085-5AA93B39B59E}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29710565-1A36-454F-AF6B-B68F86CBBE16}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F37BA7D8-C15A-43F5-BBC7-C053892C007E}"/>
 </file>
</xml_diff>

<commit_message>
adjusted the data, and added another set of events
</commit_message>
<xml_diff>
--- a/Copy of earnings_Alnylam.xlsx
+++ b/Copy of earnings_Alnylam.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christianweissmeier/Documents/Wu_Wien/Q3/Corporate Finance/Team_Project/r-code/Corporate Finance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvos2\OneDrive\Desktop\MEGA\2. WU Wien\Semester 2\Corporate Finance\Cases\QFin_CF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDADBFF5-CC7B-C345-A62E-E6CAF93F7A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69787DA4-342E-44FF-BC86-886D9AE24F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Per</t>
   </si>
@@ -271,12 +271,30 @@
   </si>
   <si>
     <t>Neutral</t>
+  </si>
+  <si>
+    <t>Amount of Good's</t>
+  </si>
+  <si>
+    <t>Amount of Neutral's</t>
+  </si>
+  <si>
+    <t>Amount of Bad's</t>
+  </si>
+  <si>
+    <t>Good News Bound</t>
+  </si>
+  <si>
+    <t>Bad News Bound</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -770,10 +788,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="26"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -816,7 +835,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="38" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="39" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="43" builtinId="5"/>
+    <cellStyle name="Percent" xfId="43" builtinId="5"/>
     <cellStyle name="Title" xfId="40" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
@@ -838,16 +857,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>16933</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>207433</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>198967</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>294217</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,8 +889,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6756400" y="414867"/>
-          <a:ext cx="3568700" cy="711200"/>
+          <a:off x="5490633" y="2413000"/>
+          <a:ext cx="3134784" cy="698500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1219,19 +1238,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1254,7 +1274,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1275,11 +1295,17 @@
         <v>8.5057471264367759E-2</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G24" si="1">+IF(F2&gt;=0.025,"Good",IF(F2&lt;=-0.025,"Bad","Neutral"))</f>
-        <v>Good</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <f>+IF(F2&gt;=$J$2,"Good",IF(F2&lt;=$J$3,"Bad","Neutral"))</f>
+        <v>Neutral</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1300,11 +1326,17 @@
         <v>7.1923076923076916</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G3:G24" si="1">+IF(F3&gt;=$J$2,"Good",IF(F3&lt;=$J$3,"Bad","Neutral"))</f>
         <v>Good</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="3">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1329,7 +1361,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1386,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1379,7 +1411,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1403,8 +1435,15 @@
         <f t="shared" si="1"/>
         <v>Bad</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7">
+        <f>COUNTIF(G2:G24, "Good")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1428,8 +1467,15 @@
         <f t="shared" si="1"/>
         <v>Good</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J8">
+        <f>COUNTIF(G2:G24, "Bad")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1453,8 +1499,15 @@
         <f t="shared" si="1"/>
         <v>Good</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9">
+        <f>COUNTIF(G2:G24, "Neutral")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1479,7 +1532,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1504,7 +1557,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1526,10 +1579,10 @@
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
-        <v>Bad</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+        <v>Neutral</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1554,7 +1607,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -1579,7 +1632,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1604,7 +1657,7 @@
         <v>Neutral</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -1626,10 +1679,10 @@
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>Neutral</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1654,7 +1707,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -1679,7 +1732,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1704,7 +1757,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>58</v>
       </c>
@@ -1729,7 +1782,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -1754,7 +1807,7 @@
         <v>Bad</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1779,7 +1832,7 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1801,10 +1854,10 @@
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
-        <v>Good</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>Neutral</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -1829,64 +1882,64 @@
         <v>Good</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F36" s="2"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F37" s="2"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F42" s="2"/>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F43" s="2"/>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F44" s="2"/>
     </row>
   </sheetData>
@@ -1903,33 +1956,33 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>76</v>
       </c>
       <c r="C4">
         <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B4)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>78</v>
       </c>
       <c r="C5">
         <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>77</v>
       </c>
       <c r="C6">
         <f>+COUNTIF(Worksheet!$G$2:$G$24,Formula!B6)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1939,6 +1992,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006483248081D4D34083215F2A9507A283" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7e618be4f2b80e79eaadc52ea446d95c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="85942912-2c17-4d13-bcab-472c0bf30a39" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c80daec75caaa22acc5c26d2fb929cb0" ns2:_="">
     <xsd:import namespace="85942912-2c17-4d13-bcab-472c0bf30a39"/>
@@ -2082,29 +2150,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56694664-2CCF-469C-A085-5AA93B39B59E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F37BA7D8-C15A-43F5-BBC7-C053892C007E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29710565-1A36-454F-AF6B-B68F86CBBE16}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29710565-1A36-454F-AF6B-B68F86CBBE16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F37BA7D8-C15A-43F5-BBC7-C053892C007E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56694664-2CCF-469C-A085-5AA93B39B59E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="85942912-2c17-4d13-bcab-472c0bf30a39"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>